<commit_message>
Minor commit on JBM
</commit_message>
<xml_diff>
--- a/ControlUnit/ControlWords.xlsx
+++ b/ControlUnit/ControlWords.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B9AF86-D247-4785-9849-47093165320A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98A7C4D-F70E-4F91-8B24-EE835A9BFD75}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="123">
   <si>
     <t>Fetch</t>
   </si>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>scrive in R31</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>where R0 means reading (RD1 = 1) register r0</t>
   </si>
 </sst>
 </file>
@@ -875,10 +881,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD595A4D-8C50-4DCE-A8ED-58F97BE824DB}">
-  <dimension ref="A1:S61"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44:E49"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,8 +952,8 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="7">
-        <v>0</v>
+      <c r="F2" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>32</v>
@@ -999,8 +1005,8 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="7">
-        <v>0</v>
+      <c r="F3" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>32</v>
@@ -1052,8 +1058,8 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="7">
-        <v>0</v>
+      <c r="F4" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>32</v>
@@ -1105,8 +1111,8 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="7">
-        <v>0</v>
+      <c r="F5" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>32</v>
@@ -1158,8 +1164,8 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="7">
-        <v>0</v>
+      <c r="F6" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>32</v>
@@ -1211,8 +1217,8 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="7">
-        <v>0</v>
+      <c r="F7" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>32</v>
@@ -1264,8 +1270,8 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="7">
-        <v>0</v>
+      <c r="F8" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>32</v>
@@ -1317,8 +1323,8 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="7">
-        <v>0</v>
+      <c r="F9" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>32</v>
@@ -1370,8 +1376,8 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="7">
-        <v>0</v>
+      <c r="F10" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>32</v>
@@ -1423,8 +1429,8 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="7">
-        <v>0</v>
+      <c r="F11" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>32</v>
@@ -1476,8 +1482,8 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="7">
-        <v>0</v>
+      <c r="F12" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>32</v>
@@ -1529,8 +1535,8 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="7">
-        <v>0</v>
+      <c r="F13" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>32</v>
@@ -1582,8 +1588,8 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" s="7">
-        <v>0</v>
+      <c r="F14" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>32</v>
@@ -1635,8 +1641,8 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" s="7">
-        <v>0</v>
+      <c r="F15" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>32</v>
@@ -1688,8 +1694,8 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" s="7">
-        <v>0</v>
+      <c r="F16" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>32</v>
@@ -1741,8 +1747,8 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17" s="7">
-        <v>0</v>
+      <c r="F17" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>32</v>
@@ -1794,8 +1800,8 @@
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" s="7">
-        <v>0</v>
+      <c r="F18" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>32</v>
@@ -1847,8 +1853,8 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" s="7">
-        <v>0</v>
+      <c r="F19" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>32</v>
@@ -1900,8 +1906,8 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" s="7">
-        <v>0</v>
+      <c r="F20" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>32</v>
@@ -1953,8 +1959,8 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21" s="7">
-        <v>0</v>
+      <c r="F21" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>32</v>
@@ -2006,8 +2012,8 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22" s="7">
-        <v>0</v>
+      <c r="F22" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>32</v>
@@ -2059,8 +2065,8 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23" s="7">
-        <v>0</v>
+      <c r="F23" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>32</v>
@@ -2112,8 +2118,8 @@
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24" s="7">
-        <v>0</v>
+      <c r="F24" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>88</v>
@@ -2165,8 +2171,8 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" s="7">
-        <v>0</v>
+      <c r="F25" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>32</v>
@@ -2218,8 +2224,8 @@
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26" s="7">
-        <v>0</v>
+      <c r="F26" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>88</v>
@@ -2271,8 +2277,8 @@
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="F27" s="7">
-        <v>0</v>
+      <c r="F27" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>32</v>
@@ -2324,8 +2330,8 @@
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="F28" s="7">
-        <v>0</v>
+      <c r="F28" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>32</v>
@@ -2377,8 +2383,8 @@
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29" s="7">
-        <v>0</v>
+      <c r="F29" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>32</v>
@@ -2430,8 +2436,8 @@
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="F30" s="7">
-        <v>0</v>
+      <c r="F30" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>32</v>
@@ -2483,8 +2489,8 @@
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31" s="7">
-        <v>0</v>
+      <c r="F31" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>32</v>
@@ -2536,8 +2542,8 @@
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32" s="7">
-        <v>0</v>
+      <c r="F32" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>32</v>
@@ -2589,8 +2595,8 @@
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="F33" s="7">
-        <v>0</v>
+      <c r="F33" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>32</v>
@@ -2642,8 +2648,8 @@
       <c r="E34">
         <v>1</v>
       </c>
-      <c r="F34" s="7">
-        <v>0</v>
+      <c r="F34" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>32</v>
@@ -2695,8 +2701,8 @@
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="F35" s="7">
-        <v>0</v>
+      <c r="F35" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>32</v>
@@ -2748,8 +2754,8 @@
       <c r="E36">
         <v>1</v>
       </c>
-      <c r="F36" s="7">
-        <v>0</v>
+      <c r="F36" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>32</v>
@@ -2801,8 +2807,8 @@
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37" s="7">
-        <v>0</v>
+      <c r="F37" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>32</v>
@@ -2854,8 +2860,8 @@
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="F38" s="7">
-        <v>0</v>
+      <c r="F38" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>32</v>
@@ -2907,8 +2913,8 @@
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="F39" s="7">
-        <v>0</v>
+      <c r="F39" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G39">
         <v>10</v>
@@ -2960,8 +2966,8 @@
       <c r="E40">
         <v>1</v>
       </c>
-      <c r="F40" s="7">
-        <v>0</v>
+      <c r="F40" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G40">
         <v>10</v>
@@ -3013,8 +3019,8 @@
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41" s="7">
-        <v>0</v>
+      <c r="F41" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G41">
         <v>10</v>
@@ -3066,8 +3072,8 @@
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="F42" s="7">
-        <v>0</v>
+      <c r="F42" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G42">
         <v>10</v>
@@ -3119,8 +3125,8 @@
       <c r="E43">
         <v>1</v>
       </c>
-      <c r="F43" s="7">
-        <v>0</v>
+      <c r="F43" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G43">
         <v>10</v>
@@ -3172,8 +3178,8 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44" s="7">
-        <v>0</v>
+      <c r="F44" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>98</v>
@@ -3225,8 +3231,8 @@
       <c r="E45">
         <v>1</v>
       </c>
-      <c r="F45" s="7">
-        <v>0</v>
+      <c r="F45" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>98</v>
@@ -3281,8 +3287,8 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46" s="7">
-        <v>0</v>
+      <c r="F46" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>32</v>
@@ -3334,8 +3340,8 @@
       <c r="E47">
         <v>1</v>
       </c>
-      <c r="F47" s="7">
-        <v>0</v>
+      <c r="F47" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>32</v>
@@ -3390,8 +3396,8 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48" s="7">
-        <v>0</v>
+      <c r="F48" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>88</v>
@@ -3443,8 +3449,8 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49" s="7">
-        <v>0</v>
+      <c r="F49" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>88</v>
@@ -3496,8 +3502,8 @@
       <c r="E50">
         <v>1</v>
       </c>
-      <c r="F50" s="7">
-        <v>0</v>
+      <c r="F50" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>88</v>
@@ -3549,8 +3555,8 @@
       <c r="E51">
         <v>1</v>
       </c>
-      <c r="F51" s="7">
-        <v>0</v>
+      <c r="F51" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>88</v>
@@ -3602,8 +3608,8 @@
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52" s="7">
-        <v>0</v>
+      <c r="F52" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G52" s="7" t="s">
         <v>88</v>
@@ -3655,8 +3661,8 @@
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53" s="7">
-        <v>0</v>
+      <c r="F53" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>88</v>
@@ -3708,8 +3714,8 @@
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54" s="7">
-        <v>0</v>
+      <c r="F54" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G54" s="7" t="s">
         <v>88</v>
@@ -3761,8 +3767,8 @@
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55" s="7">
-        <v>0</v>
+      <c r="F55" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G55" s="7" t="s">
         <v>88</v>
@@ -3814,8 +3820,8 @@
       <c r="E56">
         <v>0</v>
       </c>
-      <c r="F56" s="7">
-        <v>0</v>
+      <c r="F56" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>88</v>
@@ -3867,8 +3873,8 @@
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57" s="7">
-        <v>0</v>
+      <c r="F57" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>88</v>
@@ -3911,17 +3917,17 @@
       <c r="A58" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
+      <c r="C58" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58" t="s">
+        <v>121</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58" s="7">
-        <v>0</v>
+      <c r="F58" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G58" s="7" t="s">
         <v>32</v>
@@ -3964,8 +3970,8 @@
       <c r="A59" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C59">
-        <v>0</v>
+      <c r="C59" t="s">
+        <v>121</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -3973,8 +3979,8 @@
       <c r="E59">
         <v>1</v>
       </c>
-      <c r="F59" s="7">
-        <v>0</v>
+      <c r="F59" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>88</v>
@@ -4017,17 +4023,17 @@
       <c r="A60" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
+      <c r="C60" t="s">
+        <v>121</v>
+      </c>
+      <c r="D60" t="s">
+        <v>121</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="F60" s="7">
-        <v>0</v>
+      <c r="F60" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G60" s="7" t="s">
         <v>32</v>
@@ -4070,17 +4076,17 @@
       <c r="A61" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
+      <c r="C61" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61" t="s">
+        <v>121</v>
       </c>
       <c r="E61">
         <v>1</v>
       </c>
-      <c r="F61" s="7">
-        <v>0</v>
+      <c r="F61" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>32</v>
@@ -4117,6 +4123,11 @@
       </c>
       <c r="R61">
         <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Decode 0.6, JBM 0.3
</commit_message>
<xml_diff>
--- a/ControlUnit/ControlWords.xlsx
+++ b/ControlUnit/ControlWords.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98A7C4D-F70E-4F91-8B24-EE835A9BFD75}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F64E4C-9991-4B92-9A6F-2269EDB95694}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="122">
   <si>
     <t>Fetch</t>
   </si>
@@ -384,9 +384,6 @@
   </si>
   <si>
     <t>scrive in R31</t>
-  </si>
-  <si>
-    <t>R0</t>
   </si>
   <si>
     <t>where R0 means reading (RD1 = 1) register r0</t>
@@ -883,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD595A4D-8C50-4DCE-A8ED-58F97BE824DB}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3917,11 +3914,11 @@
       <c r="A58" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C58" t="s">
-        <v>121</v>
-      </c>
-      <c r="D58" t="s">
-        <v>121</v>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -3970,8 +3967,8 @@
       <c r="A59" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C59" t="s">
-        <v>121</v>
+      <c r="C59">
+        <v>0</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -4023,11 +4020,11 @@
       <c r="A60" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C60" t="s">
-        <v>121</v>
-      </c>
-      <c r="D60" t="s">
-        <v>121</v>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -4076,11 +4073,11 @@
       <c r="A61" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C61" t="s">
-        <v>121</v>
-      </c>
-      <c r="D61" t="s">
-        <v>121</v>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -4127,7 +4124,7 @@
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Instruction LAHI LAHIU added
</commit_message>
<xml_diff>
--- a/ControlUnit/ControlWords.xlsx
+++ b/ControlUnit/ControlWords.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F64E4C-9991-4B92-9A6F-2269EDB95694}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2D34B2-48DB-4036-967E-481B46996B19}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="128">
   <si>
     <t>Fetch</t>
   </si>
@@ -386,14 +386,32 @@
     <t>scrive in R31</t>
   </si>
   <si>
-    <t>where R0 means reading (RD1 = 1) register r0</t>
+    <t>lahi</t>
+  </si>
+  <si>
+    <t>lahiu</t>
+  </si>
+  <si>
+    <t>001010</t>
+  </si>
+  <si>
+    <t>l'operando Imm entra in ExOpA, da gestire il data forwording</t>
+  </si>
+  <si>
+    <t>UsePC x2</t>
+  </si>
+  <si>
+    <t>UseImm</t>
+  </si>
+  <si>
+    <t>ReversOp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +430,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -468,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -484,6 +510,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -878,15 +908,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD595A4D-8C50-4DCE-A8ED-58F97BE824DB}">
-  <dimension ref="A1:S65"/>
+  <dimension ref="A1:V64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
@@ -903,40 +933,49 @@
         <v>20</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -955,26 +994,20 @@
       <c r="G2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
+      <c r="L2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -982,14 +1015,23 @@
       <c r="P2">
         <v>0</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>97</v>
+      <c r="Q2">
+        <v>0</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1008,26 +1050,20 @@
       <c r="G3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
+      <c r="L3" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -1035,14 +1071,23 @@
       <c r="P3">
         <v>0</v>
       </c>
-      <c r="Q3" s="7" t="s">
-        <v>97</v>
+      <c r="Q3">
+        <v>0</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -1061,26 +1106,20 @@
       <c r="G4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
+      <c r="L4" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1088,14 +1127,23 @@
       <c r="P4">
         <v>0</v>
       </c>
-      <c r="Q4" s="7" t="s">
-        <v>97</v>
+      <c r="Q4">
+        <v>0</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -1114,26 +1162,20 @@
       <c r="G5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
+      <c r="L5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1141,14 +1183,23 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5" s="7" t="s">
-        <v>97</v>
+      <c r="Q5">
+        <v>0</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1167,26 +1218,20 @@
       <c r="G6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
+      <c r="L6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -1194,14 +1239,23 @@
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="Q6" s="7" t="s">
-        <v>97</v>
+      <c r="Q6">
+        <v>0</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -1220,26 +1274,20 @@
       <c r="G7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
+      <c r="L7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -1247,14 +1295,23 @@
       <c r="P7">
         <v>0</v>
       </c>
-      <c r="Q7" s="7" t="s">
-        <v>97</v>
+      <c r="Q7">
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1273,26 +1330,20 @@
       <c r="G8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
+      <c r="L8" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -1300,14 +1351,23 @@
       <c r="P8">
         <v>0</v>
       </c>
-      <c r="Q8" s="7" t="s">
-        <v>97</v>
+      <c r="Q8">
+        <v>0</v>
       </c>
       <c r="R8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -1326,26 +1386,20 @@
       <c r="G9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
+      <c r="L9" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -1353,14 +1407,23 @@
       <c r="P9">
         <v>0</v>
       </c>
-      <c r="Q9" s="7" t="s">
-        <v>97</v>
+      <c r="Q9">
+        <v>0</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -1379,26 +1442,20 @@
       <c r="G10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
+      <c r="L10" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1406,14 +1463,23 @@
       <c r="P10">
         <v>0</v>
       </c>
-      <c r="Q10" s="7" t="s">
-        <v>97</v>
+      <c r="Q10">
+        <v>0</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -1432,26 +1498,20 @@
       <c r="G11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
+      <c r="L11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -1459,14 +1519,23 @@
       <c r="P11">
         <v>0</v>
       </c>
-      <c r="Q11" s="7" t="s">
-        <v>97</v>
+      <c r="Q11">
+        <v>0</v>
       </c>
       <c r="R11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -1485,26 +1554,20 @@
       <c r="G12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
+      <c r="L12" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -1512,14 +1575,23 @@
       <c r="P12">
         <v>0</v>
       </c>
-      <c r="Q12" s="7" t="s">
-        <v>97</v>
+      <c r="Q12">
+        <v>0</v>
       </c>
       <c r="R12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -1538,26 +1610,20 @@
       <c r="G13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
+      <c r="L13" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1565,14 +1631,23 @@
       <c r="P13">
         <v>0</v>
       </c>
-      <c r="Q13" s="7" t="s">
-        <v>97</v>
+      <c r="Q13">
+        <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
@@ -1591,26 +1666,20 @@
       <c r="G14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
+      <c r="L14" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -1618,14 +1687,23 @@
       <c r="P14">
         <v>0</v>
       </c>
-      <c r="Q14" s="7" t="s">
-        <v>97</v>
+      <c r="Q14">
+        <v>0</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1644,26 +1722,20 @@
       <c r="G15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
+      <c r="L15" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -1671,14 +1743,23 @@
       <c r="P15">
         <v>0</v>
       </c>
-      <c r="Q15" s="7" t="s">
-        <v>97</v>
+      <c r="Q15">
+        <v>0</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
@@ -1697,26 +1778,20 @@
       <c r="G16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
+      <c r="L16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -1724,14 +1799,23 @@
       <c r="P16">
         <v>0</v>
       </c>
-      <c r="Q16" s="7" t="s">
-        <v>97</v>
+      <c r="Q16">
+        <v>0</v>
       </c>
       <c r="R16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -1750,26 +1834,20 @@
       <c r="G17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
+      <c r="L17" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1777,14 +1855,23 @@
       <c r="P17">
         <v>0</v>
       </c>
-      <c r="Q17" s="7" t="s">
-        <v>97</v>
+      <c r="Q17">
+        <v>0</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1803,26 +1890,20 @@
       <c r="G18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
+      <c r="L18" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1830,14 +1911,23 @@
       <c r="P18">
         <v>0</v>
       </c>
-      <c r="Q18" s="7" t="s">
-        <v>97</v>
+      <c r="Q18">
+        <v>0</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>48</v>
       </c>
@@ -1856,26 +1946,20 @@
       <c r="G19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
+      <c r="L19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1883,14 +1967,23 @@
       <c r="P19">
         <v>0</v>
       </c>
-      <c r="Q19" s="7" t="s">
-        <v>97</v>
+      <c r="Q19">
+        <v>0</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>49</v>
       </c>
@@ -1909,26 +2002,20 @@
       <c r="G20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
+      <c r="L20" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1936,14 +2023,23 @@
       <c r="P20">
         <v>0</v>
       </c>
-      <c r="Q20" s="7" t="s">
-        <v>97</v>
+      <c r="Q20">
+        <v>0</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
@@ -1962,26 +2058,20 @@
       <c r="G21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
+      <c r="L21" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1989,14 +2079,23 @@
       <c r="P21">
         <v>0</v>
       </c>
-      <c r="Q21" s="7" t="s">
-        <v>97</v>
+      <c r="Q21">
+        <v>0</v>
       </c>
       <c r="R21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
@@ -2015,26 +2114,20 @@
       <c r="G22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
+      <c r="L22" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -2042,14 +2135,23 @@
       <c r="P22">
         <v>0</v>
       </c>
-      <c r="Q22" s="7" t="s">
-        <v>97</v>
+      <c r="Q22">
+        <v>0</v>
       </c>
       <c r="R22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
@@ -2068,26 +2170,20 @@
       <c r="G23" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I23" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
+      <c r="L23" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -2095,14 +2191,23 @@
       <c r="P23">
         <v>0</v>
       </c>
-      <c r="Q23" s="7" t="s">
-        <v>97</v>
+      <c r="Q23">
+        <v>0</v>
       </c>
       <c r="R23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>68</v>
       </c>
@@ -2121,26 +2226,20 @@
       <c r="G24" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
+      <c r="L24" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -2148,14 +2247,23 @@
       <c r="P24">
         <v>0</v>
       </c>
-      <c r="Q24" s="7" t="s">
-        <v>97</v>
+      <c r="Q24">
+        <v>0</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>69</v>
       </c>
@@ -2174,26 +2282,20 @@
       <c r="G25" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
+      <c r="L25" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -2201,14 +2303,23 @@
       <c r="P25">
         <v>0</v>
       </c>
-      <c r="Q25" s="7" t="s">
-        <v>97</v>
+      <c r="Q25">
+        <v>0</v>
       </c>
       <c r="R25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>70</v>
       </c>
@@ -2227,26 +2338,20 @@
       <c r="G26" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I26" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
+      <c r="L26" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -2254,14 +2359,23 @@
       <c r="P26">
         <v>0</v>
       </c>
-      <c r="Q26" s="7" t="s">
-        <v>97</v>
+      <c r="Q26">
+        <v>0</v>
       </c>
       <c r="R26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>71</v>
       </c>
@@ -2280,26 +2394,20 @@
       <c r="G27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I27" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
+      <c r="L27" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -2307,14 +2415,23 @@
       <c r="P27">
         <v>0</v>
       </c>
-      <c r="Q27" s="7" t="s">
-        <v>97</v>
+      <c r="Q27">
+        <v>0</v>
       </c>
       <c r="R27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>72</v>
       </c>
@@ -2333,26 +2450,20 @@
       <c r="G28" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I28" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
+      <c r="L28" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28">
         <v>0</v>
@@ -2360,14 +2471,23 @@
       <c r="P28">
         <v>0</v>
       </c>
-      <c r="Q28" s="7" t="s">
-        <v>97</v>
+      <c r="Q28">
+        <v>0</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>73</v>
       </c>
@@ -2386,26 +2506,20 @@
       <c r="G29" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I29" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
+      <c r="L29" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O29">
         <v>0</v>
@@ -2413,14 +2527,23 @@
       <c r="P29">
         <v>0</v>
       </c>
-      <c r="Q29" s="7" t="s">
-        <v>97</v>
+      <c r="Q29">
+        <v>0</v>
       </c>
       <c r="R29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -2439,26 +2562,20 @@
       <c r="G30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I30" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>0</v>
+      <c r="L30" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30">
         <v>0</v>
@@ -2466,14 +2583,23 @@
       <c r="P30">
         <v>0</v>
       </c>
-      <c r="Q30" s="7" t="s">
-        <v>97</v>
+      <c r="Q30">
+        <v>0</v>
       </c>
       <c r="R30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>75</v>
       </c>
@@ -2492,26 +2618,20 @@
       <c r="G31" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I31" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
+      <c r="L31" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O31">
         <v>0</v>
@@ -2519,14 +2639,23 @@
       <c r="P31">
         <v>0</v>
       </c>
-      <c r="Q31" s="7" t="s">
-        <v>97</v>
+      <c r="Q31">
+        <v>0</v>
       </c>
       <c r="R31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>76</v>
       </c>
@@ -2545,26 +2674,20 @@
       <c r="G32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H32" s="7" t="s">
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I32" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32">
-        <v>0</v>
+      <c r="L32" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32">
         <v>0</v>
@@ -2572,14 +2695,23 @@
       <c r="P32">
         <v>0</v>
       </c>
-      <c r="Q32" s="7" t="s">
-        <v>97</v>
+      <c r="Q32">
+        <v>0</v>
       </c>
       <c r="R32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>77</v>
       </c>
@@ -2598,26 +2730,20 @@
       <c r="G33" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I33" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <v>0</v>
+      <c r="L33" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O33">
         <v>0</v>
@@ -2625,14 +2751,23 @@
       <c r="P33">
         <v>0</v>
       </c>
-      <c r="Q33" s="7" t="s">
-        <v>97</v>
+      <c r="Q33">
+        <v>0</v>
       </c>
       <c r="R33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
@@ -2651,26 +2786,20 @@
       <c r="G34" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I34" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="M34">
-        <v>0</v>
+      <c r="L34" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O34">
         <v>0</v>
@@ -2678,14 +2807,23 @@
       <c r="P34">
         <v>0</v>
       </c>
-      <c r="Q34" s="7" t="s">
-        <v>97</v>
+      <c r="Q34">
+        <v>0</v>
       </c>
       <c r="R34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>79</v>
       </c>
@@ -2704,26 +2842,20 @@
       <c r="G35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I35" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
+      <c r="L35" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O35">
         <v>0</v>
@@ -2731,14 +2863,23 @@
       <c r="P35">
         <v>0</v>
       </c>
-      <c r="Q35" s="7" t="s">
-        <v>97</v>
+      <c r="Q35">
+        <v>0</v>
       </c>
       <c r="R35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>80</v>
       </c>
@@ -2757,26 +2898,20 @@
       <c r="G36" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H36" s="7" t="s">
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-      <c r="M36">
-        <v>0</v>
+      <c r="L36" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -2784,14 +2919,23 @@
       <c r="P36">
         <v>0</v>
       </c>
-      <c r="Q36" s="7" t="s">
-        <v>97</v>
+      <c r="Q36">
+        <v>0</v>
       </c>
       <c r="R36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>81</v>
       </c>
@@ -2810,26 +2954,20 @@
       <c r="G37" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
+      <c r="L37" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O37">
         <v>0</v>
@@ -2837,14 +2975,23 @@
       <c r="P37">
         <v>0</v>
       </c>
-      <c r="Q37" s="7" t="s">
-        <v>97</v>
+      <c r="Q37">
+        <v>0</v>
       </c>
       <c r="R37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>82</v>
       </c>
@@ -2863,26 +3010,20 @@
       <c r="G38" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H38" s="7" t="s">
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K38">
-        <v>1</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
+      <c r="L38" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M38" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O38">
         <v>0</v>
@@ -2890,14 +3031,23 @@
       <c r="P38">
         <v>0</v>
       </c>
-      <c r="Q38" s="7" t="s">
-        <v>97</v>
+      <c r="Q38">
+        <v>0</v>
       </c>
       <c r="R38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>83</v>
       </c>
@@ -2916,26 +3066,17 @@
       <c r="G39">
         <v>10</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="K39" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I39" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J39" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K39">
-        <v>1</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39">
-        <v>0</v>
+      <c r="L39" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O39">
         <v>0</v>
@@ -2943,14 +3084,23 @@
       <c r="P39">
         <v>0</v>
       </c>
-      <c r="Q39" s="7" t="s">
-        <v>97</v>
+      <c r="Q39">
+        <v>0</v>
       </c>
       <c r="R39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>84</v>
       </c>
@@ -2969,26 +3119,17 @@
       <c r="G40">
         <v>10</v>
       </c>
-      <c r="H40" s="7" t="s">
+      <c r="K40" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I40" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
+      <c r="L40" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O40">
         <v>0</v>
@@ -2996,14 +3137,23 @@
       <c r="P40">
         <v>0</v>
       </c>
-      <c r="Q40" s="7" t="s">
-        <v>97</v>
+      <c r="Q40">
+        <v>0</v>
       </c>
       <c r="R40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>85</v>
       </c>
@@ -3022,26 +3172,17 @@
       <c r="G41">
         <v>10</v>
       </c>
-      <c r="H41" s="7" t="s">
+      <c r="K41" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I41" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K41">
-        <v>1</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
+      <c r="L41" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O41">
         <v>0</v>
@@ -3049,14 +3190,23 @@
       <c r="P41">
         <v>0</v>
       </c>
-      <c r="Q41" s="7" t="s">
-        <v>97</v>
+      <c r="Q41">
+        <v>0</v>
       </c>
       <c r="R41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>86</v>
       </c>
@@ -3075,26 +3225,17 @@
       <c r="G42">
         <v>10</v>
       </c>
-      <c r="H42" s="7" t="s">
+      <c r="K42" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I42" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K42">
-        <v>1</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
+      <c r="L42" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O42">
         <v>0</v>
@@ -3102,14 +3243,23 @@
       <c r="P42">
         <v>0</v>
       </c>
-      <c r="Q42" s="7" t="s">
-        <v>97</v>
+      <c r="Q42">
+        <v>0</v>
       </c>
       <c r="R42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S42">
+        <v>0</v>
+      </c>
+      <c r="T42" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>87</v>
       </c>
@@ -3128,26 +3278,17 @@
       <c r="G43">
         <v>10</v>
       </c>
-      <c r="H43" s="7" t="s">
+      <c r="K43" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I43" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K43">
-        <v>1</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
+      <c r="L43" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O43">
         <v>0</v>
@@ -3155,14 +3296,23 @@
       <c r="P43">
         <v>0</v>
       </c>
-      <c r="Q43" s="7" t="s">
-        <v>97</v>
+      <c r="Q43">
+        <v>0</v>
       </c>
       <c r="R43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>90</v>
       </c>
@@ -3181,26 +3331,20 @@
       <c r="G44" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H44" s="7" t="s">
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I44" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J44" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K44">
-        <v>1</v>
-      </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
+      <c r="L44" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O44">
         <v>0</v>
@@ -3208,14 +3352,23 @@
       <c r="P44">
         <v>0</v>
       </c>
-      <c r="Q44" s="7" t="s">
-        <v>97</v>
+      <c r="Q44">
+        <v>0</v>
       </c>
       <c r="R44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>91</v>
       </c>
@@ -3234,26 +3387,20 @@
       <c r="G45" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H45" s="7" t="s">
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I45" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J45" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K45">
-        <v>1</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45">
-        <v>0</v>
+      <c r="L45" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O45">
         <v>0</v>
@@ -3261,17 +3408,26 @@
       <c r="P45">
         <v>0</v>
       </c>
-      <c r="Q45" s="7" t="s">
-        <v>97</v>
+      <c r="Q45">
+        <v>0</v>
       </c>
       <c r="R45">
         <v>0</v>
       </c>
-      <c r="S45" s="10" t="s">
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U45">
+        <v>0</v>
+      </c>
+      <c r="V45" s="10" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>92</v>
       </c>
@@ -3290,26 +3446,20 @@
       <c r="G46" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H46" s="7" t="s">
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I46" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J46" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K46">
-        <v>1</v>
-      </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-      <c r="M46">
-        <v>0</v>
+      <c r="L46" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -3317,14 +3467,23 @@
       <c r="P46">
         <v>0</v>
       </c>
-      <c r="Q46" s="7" t="s">
-        <v>97</v>
+      <c r="Q46">
+        <v>0</v>
       </c>
       <c r="R46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>93</v>
       </c>
@@ -3343,26 +3502,20 @@
       <c r="G47" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I47" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J47" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K47">
-        <v>1</v>
-      </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-      <c r="M47">
-        <v>0</v>
+      <c r="L47" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O47">
         <v>0</v>
@@ -3370,17 +3523,26 @@
       <c r="P47">
         <v>0</v>
       </c>
-      <c r="Q47" s="7" t="s">
-        <v>97</v>
+      <c r="Q47">
+        <v>0</v>
       </c>
       <c r="R47">
         <v>0</v>
       </c>
-      <c r="S47" s="10" t="s">
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+      <c r="V47" s="10" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>99</v>
       </c>
@@ -3399,26 +3561,20 @@
       <c r="G48" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H48" s="7" t="s">
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I48" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J48" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K48">
-        <v>1</v>
-      </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-      <c r="M48">
-        <v>0</v>
+      <c r="L48" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O48">
         <v>0</v>
@@ -3426,14 +3582,23 @@
       <c r="P48">
         <v>0</v>
       </c>
-      <c r="Q48" s="7" t="s">
-        <v>97</v>
+      <c r="Q48">
+        <v>0</v>
       </c>
       <c r="R48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S48">
+        <v>0</v>
+      </c>
+      <c r="T48" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>100</v>
       </c>
@@ -3452,26 +3617,20 @@
       <c r="G49" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H49" s="7" t="s">
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I49" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J49" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K49">
-        <v>1</v>
-      </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49">
-        <v>0</v>
+      <c r="L49" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M49" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49">
         <v>0</v>
@@ -3479,14 +3638,23 @@
       <c r="P49">
         <v>0</v>
       </c>
-      <c r="Q49" s="7" t="s">
-        <v>97</v>
+      <c r="Q49">
+        <v>0</v>
       </c>
       <c r="R49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>101</v>
       </c>
@@ -3505,41 +3673,44 @@
       <c r="G50" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H50" s="7" t="s">
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I50" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J50" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K50">
-        <v>1</v>
-      </c>
-      <c r="L50">
-        <v>1</v>
-      </c>
-      <c r="M50">
-        <v>0</v>
+      <c r="L50" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O50">
         <v>1</v>
       </c>
       <c r="P50">
-        <v>1</v>
-      </c>
-      <c r="Q50" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="R50" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+      <c r="S50">
+        <v>1</v>
+      </c>
+      <c r="T50" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="U50" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>109</v>
       </c>
@@ -3558,41 +3729,44 @@
       <c r="G51" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H51" s="7" t="s">
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I51" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J51" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K51">
-        <v>1</v>
-      </c>
-      <c r="L51">
-        <v>1</v>
-      </c>
-      <c r="M51">
-        <v>0</v>
+      <c r="L51" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O51">
         <v>1</v>
       </c>
       <c r="P51">
-        <v>1</v>
-      </c>
-      <c r="Q51" s="8" t="s">
-        <v>96</v>
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
       </c>
       <c r="R51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="S51">
+        <v>1</v>
+      </c>
+      <c r="T51" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="U51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>111</v>
       </c>
@@ -3611,41 +3785,44 @@
       <c r="G52" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H52" s="7" t="s">
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I52" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J52" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K52">
-        <v>1</v>
-      </c>
-      <c r="L52">
-        <v>1</v>
-      </c>
-      <c r="M52">
-        <v>0</v>
+      <c r="L52" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O52">
         <v>1</v>
       </c>
       <c r="P52">
-        <v>1</v>
-      </c>
-      <c r="Q52" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="R52" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>1</v>
+      </c>
+      <c r="S52">
+        <v>1</v>
+      </c>
+      <c r="T52" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U52" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>112</v>
       </c>
@@ -3664,41 +3841,44 @@
       <c r="G53" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H53" s="7" t="s">
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I53" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J53" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K53">
-        <v>1</v>
-      </c>
-      <c r="L53">
-        <v>1</v>
-      </c>
-      <c r="M53">
-        <v>0</v>
+      <c r="L53" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M53" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O53">
         <v>1</v>
       </c>
       <c r="P53">
-        <v>1</v>
-      </c>
-      <c r="Q53" s="7" t="s">
-        <v>97</v>
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
       </c>
       <c r="R53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="S53">
+        <v>1</v>
+      </c>
+      <c r="T53" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>102</v>
       </c>
@@ -3717,26 +3897,20 @@
       <c r="G54" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H54" s="7" t="s">
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I54" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J54" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K54">
-        <v>1</v>
-      </c>
-      <c r="L54">
-        <v>1</v>
-      </c>
-      <c r="M54">
-        <v>0</v>
+      <c r="L54" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O54">
         <v>1</v>
@@ -3744,14 +3918,23 @@
       <c r="P54">
         <v>0</v>
       </c>
-      <c r="Q54" s="7" t="s">
-        <v>97</v>
+      <c r="Q54">
+        <v>0</v>
       </c>
       <c r="R54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>103</v>
       </c>
@@ -3770,41 +3953,44 @@
       <c r="G55" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H55" s="7" t="s">
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I55" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J55" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K55" s="10">
-        <v>0</v>
-      </c>
-      <c r="L55">
-        <v>1</v>
-      </c>
-      <c r="M55" s="10">
-        <v>1</v>
+      <c r="L55" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M55" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N55" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O55">
         <v>1</v>
       </c>
-      <c r="P55">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="7" t="s">
-        <v>97</v>
+      <c r="P55" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="10">
+        <v>1</v>
       </c>
       <c r="R55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="S55">
+        <v>0</v>
+      </c>
+      <c r="T55" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>113</v>
       </c>
@@ -3823,41 +4009,44 @@
       <c r="G56" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H56" s="7" t="s">
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I56" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J56" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K56" s="10">
-        <v>0</v>
-      </c>
-      <c r="L56">
-        <v>1</v>
-      </c>
-      <c r="M56" s="10">
-        <v>1</v>
-      </c>
-      <c r="N56">
+      <c r="L56" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="N56" s="10">
         <v>0</v>
       </c>
       <c r="O56">
         <v>1</v>
       </c>
-      <c r="P56">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="7" t="s">
-        <v>97</v>
+      <c r="P56" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q56">
+        <v>0</v>
       </c>
       <c r="R56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="S56">
+        <v>0</v>
+      </c>
+      <c r="T56" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>104</v>
       </c>
@@ -3876,25 +4065,19 @@
       <c r="G57" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H57" s="7" t="s">
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I57" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J57" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K57" s="10">
-        <v>0</v>
-      </c>
-      <c r="L57">
-        <v>1</v>
-      </c>
-      <c r="M57">
-        <v>0</v>
-      </c>
-      <c r="N57">
+      <c r="L57" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M57" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="N57" s="10">
         <v>0</v>
       </c>
       <c r="O57">
@@ -3907,10 +4090,19 @@
         <v>0</v>
       </c>
       <c r="R57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="S57">
+        <v>0</v>
+      </c>
+      <c r="T57">
+        <v>0</v>
+      </c>
+      <c r="U57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>105</v>
       </c>
@@ -3929,26 +4121,20 @@
       <c r="G58" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H58" s="7" t="s">
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I58" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J58" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K58">
-        <v>1</v>
-      </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-      <c r="M58">
-        <v>0</v>
+      <c r="L58" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M58" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O58">
         <v>0</v>
@@ -3962,8 +4148,17 @@
       <c r="R58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S58">
+        <v>0</v>
+      </c>
+      <c r="T58">
+        <v>0</v>
+      </c>
+      <c r="U58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>106</v>
       </c>
@@ -3982,26 +4177,20 @@
       <c r="G59" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H59" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I59" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J59" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K59">
-        <v>1</v>
-      </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-      <c r="M59">
-        <v>0</v>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L59" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M59" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="N59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O59">
         <v>0</v>
@@ -4015,8 +4204,17 @@
       <c r="R59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S59">
+        <v>0</v>
+      </c>
+      <c r="T59">
+        <v>0</v>
+      </c>
+      <c r="U59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>107</v>
       </c>
@@ -4035,26 +4233,20 @@
       <c r="G60" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H60" s="7" t="s">
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I60" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J60" s="8" t="s">
+      <c r="L60" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M60" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="K60">
-        <v>1</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-      <c r="M60">
-        <v>0</v>
-      </c>
       <c r="N60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O60">
         <v>0</v>
@@ -4068,8 +4260,17 @@
       <c r="R60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="S60">
+        <v>0</v>
+      </c>
+      <c r="T60">
+        <v>0</v>
+      </c>
+      <c r="U60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>108</v>
       </c>
@@ -4088,26 +4289,20 @@
       <c r="G61" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H61" s="7" t="s">
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I61" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J61" s="8" t="s">
+      <c r="L61" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M61" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K61">
-        <v>1</v>
-      </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-      <c r="M61">
-        <v>0</v>
-      </c>
       <c r="N61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O61">
         <v>0</v>
@@ -4121,10 +4316,131 @@
       <c r="R61">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
+      <c r="S61">
+        <v>0</v>
+      </c>
+      <c r="T61">
+        <v>0</v>
+      </c>
+      <c r="U61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
         <v>121</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="L62" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M62" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <v>0</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62">
+        <v>0</v>
+      </c>
+      <c r="T62">
+        <v>0</v>
+      </c>
+      <c r="U62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L63" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M63" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="N63">
+        <v>1</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63">
+        <v>0</v>
+      </c>
+      <c r="U63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A64" s="12" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready to write DLX Core VHDL
</commit_message>
<xml_diff>
--- a/ControlUnit/ControlWords.xlsx
+++ b/ControlUnit/ControlWords.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF3F627-9CD2-4F16-AE00-D4A80A7908BD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07098780-D091-4E5C-8633-4C78E0F77E1C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="132">
   <si>
     <t>Fetch</t>
   </si>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>sra+A4:R4</t>
+  </si>
+  <si>
+    <t>&lt;- Maybe should be 0?</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -496,6 +499,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -509,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -535,6 +544,7 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -931,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD595A4D-8C50-4DCE-A8ED-58F97BE824DB}">
   <dimension ref="A1:W70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="L63" sqref="L63"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="P67" sqref="P67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4502,7 +4512,7 @@
       <c r="R55" s="10">
         <v>1</v>
       </c>
-      <c r="S55">
+      <c r="S55" s="15">
         <v>1</v>
       </c>
       <c r="T55">
@@ -4567,7 +4577,7 @@
       <c r="R56">
         <v>0</v>
       </c>
-      <c r="S56">
+      <c r="S56" s="15">
         <v>1</v>
       </c>
       <c r="T56">
@@ -4632,7 +4642,7 @@
       <c r="R57">
         <v>0</v>
       </c>
-      <c r="S57">
+      <c r="S57" s="15">
         <v>1</v>
       </c>
       <c r="T57">
@@ -5040,17 +5050,23 @@
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="S67" s="15"/>
+      <c r="T67" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
         <v>128</v>
       </c>

</xml_diff>